<commit_message>
updated hulk 181 to 9.9 cgc
</commit_message>
<xml_diff>
--- a/Pricey Comics.xlsx
+++ b/Pricey Comics.xlsx
@@ -691,6 +691,9 @@
     <t>1st full appearance of Wolverine</t>
   </si>
   <si>
+    <t>9.9</t>
+  </si>
+  <si>
     <t>https://cdn.marvel.com/u/prod/marvel/i/mg/9/d0/5c93f5a6e62b7/clean.jpg</t>
   </si>
   <si>
@@ -875,9 +878,6 @@
   </si>
   <si>
     <t>1st appearance of Jason Macendale as the new Hobgoblin</t>
-  </si>
-  <si>
-    <t>9.9</t>
   </si>
   <si>
     <t>2016</t>
@@ -1448,11 +1448,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
@@ -2773,34 +2773,34 @@
       <c r="F38" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>105</v>
+      <c r="G38" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>105</v>
@@ -2809,12 +2809,12 @@
         <v>30</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>33</v>
@@ -2823,13 +2823,13 @@
         <v>171</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>105</v>
@@ -2838,27 +2838,27 @@
         <v>23</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>29</v>
@@ -2867,12 +2867,12 @@
         <v>30</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>33</v>
@@ -2881,13 +2881,13 @@
         <v>166</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>105</v>
@@ -2896,12 +2896,12 @@
         <v>30</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>33</v>
@@ -2910,13 +2910,13 @@
         <v>166</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>105</v>
@@ -2925,12 +2925,12 @@
         <v>23</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>33</v>
@@ -2939,13 +2939,13 @@
         <v>166</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>105</v>
@@ -2954,12 +2954,12 @@
         <v>30</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>33</v>
@@ -2971,10 +2971,10 @@
         <v>97</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>105</v>
@@ -2982,28 +2982,28 @@
       <c r="H45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>258</v>
+      <c r="I45" s="6" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>217</v>
@@ -3011,13 +3011,13 @@
       <c r="H46" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>263</v>
+      <c r="I46" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>33</v>
@@ -3026,13 +3026,13 @@
         <v>176</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>105</v>
@@ -3040,19 +3040,19 @@
       <c r="H47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>268</v>
+      <c r="I47" s="6" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>12</v>
@@ -3061,7 +3061,7 @@
         <v>172</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>105</v>
@@ -3070,27 +3070,27 @@
         <v>30</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>105</v>
@@ -3099,27 +3099,27 @@
         <v>112</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>105</v>
@@ -3128,12 +3128,12 @@
         <v>23</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>33</v>
@@ -3142,16 +3142,16 @@
         <v>176</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>288</v>
+        <v>226</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>289</v>
@@ -3272,7 +3272,7 @@
       <c r="H55" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="I55" s="5" t="s">
+      <c r="I55" s="6" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       <c r="H56" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I56" s="5" t="s">
+      <c r="I56" s="6" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3470,7 +3470,7 @@
         <v>347</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>288</v>
+        <v>226</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>348</v>
@@ -3533,7 +3533,7 @@
       <c r="H64" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I64" s="6" t="s">
         <v>359</v>
       </c>
     </row>
@@ -3615,7 +3615,7 @@
         <v>375</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>288</v>
+        <v>226</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>112</v>
@@ -3673,12 +3673,12 @@
         <v>385</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>288</v>
+        <v>226</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I69" s="6" t="s">
         <v>386</v>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
       <c r="H70" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="6" t="s">
         <v>391</v>
       </c>
     </row>
@@ -3794,7 +3794,7 @@
       <c r="H73" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I73" s="5" t="s">
+      <c r="I73" s="6" t="s">
         <v>406</v>
       </c>
     </row>
@@ -3852,7 +3852,7 @@
       <c r="H75" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I75" s="5" t="s">
+      <c r="I75" s="6" t="s">
         <v>415</v>
       </c>
     </row>
@@ -3881,7 +3881,7 @@
       <c r="H76" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I76" s="5" t="s">
+      <c r="I76" s="6" t="s">
         <v>420</v>
       </c>
     </row>
@@ -3910,7 +3910,7 @@
       <c r="H77" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I77" s="6" t="s">
         <v>424</v>
       </c>
     </row>
@@ -4147,7 +4147,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="6"/>
+      <c r="A86" s="5"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="7"/>
@@ -4158,7 +4158,7 @@
       <c r="I86" s="2"/>
     </row>
     <row r="87">
-      <c r="A87" s="6"/>
+      <c r="A87" s="5"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="7"/>

</xml_diff>